<commit_message>
24. Principal Component Analysis (PCA): Perform PCA and plot the explained variance.
</commit_message>
<xml_diff>
--- a/LM practice/kagle/Book1.xlsx
+++ b/LM practice/kagle/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zygimantas/DataspellProjects/LLM-practice/LM practice/kagle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942CB06C-08E8-9246-971E-A8BD13E353CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A808B8E7-A31B-CA40-9BC7-2E93993126FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19820" xr2:uid="{E4310E85-32CB-2048-A441-9CDBA9647663}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19800" xr2:uid="{E4310E85-32CB-2048-A441-9CDBA9647663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>MAE</t>
   </si>
@@ -70,9 +70,6 @@
     <t>294.1589874015218</t>
   </si>
   <si>
-    <t>Polynomial_regresion</t>
-  </si>
-  <si>
     <t>124.26886198188637</t>
   </si>
   <si>
@@ -128,6 +125,21 @@
   </si>
   <si>
     <t>393.8497333388905</t>
+  </si>
+  <si>
+    <t>Polynomial_regresion/Liner Regresion</t>
+  </si>
+  <si>
+    <t>202.8122865941629</t>
+  </si>
+  <si>
+    <t>198488.62338179824</t>
+  </si>
+  <si>
+    <t>445.5206206022323</t>
+  </si>
+  <si>
+    <t>Gardian Boosting Regresion</t>
   </si>
 </sst>
 </file>
@@ -183,9 +195,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +235,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -329,7 +341,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,7 +483,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,15 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F741E60A-EC20-5D4B-AE46-FF87B89C6CFC}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,72 +544,86 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
-        <v>30</v>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
25. Clustering: Perform K-means clustering on the dataset.
</commit_message>
<xml_diff>
--- a/LM practice/kagle/Book1.xlsx
+++ b/LM practice/kagle/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zygimantas/DataspellProjects/LLM-practice/LM practice/kagle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A808B8E7-A31B-CA40-9BC7-2E93993126FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB427263-618F-8743-8E72-050790C990BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19800" xr2:uid="{E4310E85-32CB-2048-A441-9CDBA9647663}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>MAE</t>
   </si>
@@ -140,6 +140,30 @@
   </si>
   <si>
     <t>Gardian Boosting Regresion</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbors</t>
+  </si>
+  <si>
+    <t>251.64652259473945</t>
+  </si>
+  <si>
+    <t>368727.3813827998</t>
+  </si>
+  <si>
+    <t>607.2292659142837</t>
+  </si>
+  <si>
+    <t>Support Vector Regression</t>
+  </si>
+  <si>
+    <t>11419.047297855577</t>
+  </si>
+  <si>
+    <t>384427929.8857064</t>
+  </si>
+  <si>
+    <t>19606.83375473221</t>
   </si>
 </sst>
 </file>
@@ -491,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F741E60A-EC20-5D4B-AE46-FF87B89C6CFC}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,6 +650,34 @@
         <v>33</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>